<commit_message>
end lần thứ n
</commit_message>
<xml_diff>
--- a/DoAnDiemDanh/Content/doc/SinhVien.xlsx
+++ b/DoAnDiemDanh/Content/doc/SinhVien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A30C74B-6DFE-47EA-A60D-2252A6EC9716}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73FEE3F-2664-42F4-9911-C9C1026C4080}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="804" windowWidth="17268" windowHeight="11004" xr2:uid="{E0489E6B-10AA-49E2-85A2-EA6CC050E602}"/>
+    <workbookView xWindow="3528" yWindow="564" windowWidth="17268" windowHeight="11004" xr2:uid="{E0489E6B-10AA-49E2-85A2-EA6CC050E602}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>Lê Văn Duy</t>
   </si>
   <si>
-    <t>Trương Văn Hoàng</t>
-  </si>
-  <si>
     <t>60.CNTT-1</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>59.CNTT-3</t>
+  </si>
+  <si>
+    <t>Nguyễn Xuân Huy</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,13 +575,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>9</v>
@@ -596,19 +596,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -629,7 +629,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -650,7 +650,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -659,19 +659,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -680,7 +680,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -692,7 +692,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -701,7 +701,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
@@ -713,7 +713,7 @@
         <v>9</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -722,19 +722,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -743,19 +743,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -764,19 +764,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G11" s="1"/>
     </row>

</xml_diff>